<commit_message>
Add initial project structure and content for environmental assessment
- Created chapters for each phase of the project: Preparation, Formulation and Evaluation, Operation, and Abandonment.
- Added tables and subsections detailing regulatory requirements and obligations.
- Included figures such as logos and banners for branding.
- Established a preamble and settings for LaTeX document formatting.
- Implemented a script for compiling references and generating the final PDF.
- Added a license file for project distribution.
</commit_message>
<xml_diff>
--- a/LaTex/16th-Semester/Análisis Financiero/Caso Flujo de Caja.xlsx
+++ b/LaTex/16th-Semester/Análisis Financiero/Caso Flujo de Caja.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/youngermaster/GitHub/Youngermaster/EAFIT-Notes/LaTex/16th-Semester/Análisis Financiero/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FC5D89-088C-FC43-AC29-1E63EBA9D816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71694A87-7154-A449-8AF8-0DE65B912993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{9767BE9B-C2AB-F748-A5E6-BD8DD22E60EE}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" activeTab="1" xr2:uid="{9767BE9B-C2AB-F748-A5E6-BD8DD22E60EE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Flujo de Caja" sheetId="1" r:id="rId1"/>
+    <sheet name="Flujo de Caja Inversionista" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -111,8 +112,84 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Juan Manuel Young Hoyos</author>
+  </authors>
+  <commentList>
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{62841BE4-E1A3-4246-B8D7-8E68489005DE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Juan Manuel Young Hoyos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Venta de la infraestructura</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{716BD10F-E6F9-0247-BFE2-1DFFFCBE4D1D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Juan Manuel Young Hoyos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Después de 40.000 Toneladas se nos hace un descuento del 10%</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
   <si>
     <t>Períodos</t>
   </si>
@@ -210,6 +287,12 @@
   <si>
     <t>Valor en
 Libros</t>
+  </si>
+  <si>
+    <t>Intereses</t>
+  </si>
+  <si>
+    <t>UAII</t>
   </si>
 </sst>
 </file>
@@ -332,9 +415,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -342,18 +422,21 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="42" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency [0]" xfId="1" builtinId="7"/>
@@ -691,7 +774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A41CDED-7692-7448-8F9E-C653C7ED6954}">
   <dimension ref="A2:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="200" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
@@ -777,16 +860,16 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -794,23 +877,23 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <f>D3*D4</f>
         <v>51000000</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <f t="shared" ref="E6:G6" si="0">E3*E4</f>
         <v>57000000</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <f t="shared" si="0"/>
         <v>79800000</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <f t="shared" si="0"/>
         <v>79800000</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <f>H3*H4</f>
         <v>79800000</v>
       </c>
@@ -821,74 +904,74 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3">
         <v>128000000</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="9">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="8">
         <f t="shared" ref="D8:H8" si="1">SUM(D6:D7)</f>
         <v>51000000</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <f t="shared" si="1"/>
         <v>57000000</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <f t="shared" si="1"/>
         <v>79800000</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <f t="shared" si="1"/>
         <v>79800000</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <f t="shared" si="1"/>
         <v>207800000</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>1500000</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3">
         <v>5000000</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>5000000</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>6500000</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>6500000</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>6500000</v>
       </c>
     </row>
@@ -896,39 +979,39 @@
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>150</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3">
         <f>$B$12*D3</f>
         <v>4500000</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <f t="shared" ref="E12:H12" si="2">$B$12*E3</f>
         <v>4500000</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <f t="shared" si="2"/>
         <v>6300000</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <f t="shared" si="2"/>
         <v>6300000</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <f t="shared" si="2"/>
         <v>6300000</v>
       </c>
@@ -937,27 +1020,27 @@
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>200</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3">
         <f>D3*$B$13*IF(D3&gt;40000,90%,100%)</f>
         <v>6000000</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <f t="shared" ref="E13:H13" si="3">E3*$B$13*IF(E3&gt;40000,90%,100%)</f>
         <v>6000000</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <f t="shared" si="3"/>
         <v>7560000</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <f t="shared" si="3"/>
         <v>7560000</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <f t="shared" si="3"/>
         <v>7560000</v>
       </c>
@@ -966,27 +1049,27 @@
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>80</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3">
         <f>$B$14*D3</f>
         <v>2400000</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <f t="shared" ref="E14:H14" si="4">$B$14*E3</f>
         <v>2400000</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <f t="shared" si="4"/>
         <v>3360000</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <f t="shared" si="4"/>
         <v>3360000</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <f t="shared" si="4"/>
         <v>3360000</v>
       </c>
@@ -995,23 +1078,23 @@
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>1500000</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3">
         <v>1500000</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>1500000</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>1500000</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>1500000</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <v>1500000</v>
       </c>
     </row>
@@ -1019,27 +1102,27 @@
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>0.03</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3">
         <f>$B$16*D6</f>
         <v>1530000</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <f t="shared" ref="E16:H16" si="5">$B$16*E6</f>
         <v>1710000</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <f t="shared" si="5"/>
         <v>2394000</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <f t="shared" si="5"/>
         <v>2394000</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <f t="shared" si="5"/>
         <v>2394000</v>
       </c>
@@ -1048,63 +1131,63 @@
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4">
+      <c r="B17" s="5"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3">
         <v>1200000</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>1200000</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>1500000</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>1500000</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <v>1500000</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9">
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8">
         <f t="shared" ref="D18" si="6">SUM(D10:D17)</f>
         <v>22130000</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <f t="shared" ref="E18" si="7">SUM(E10:E17)</f>
         <v>22310000</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <f t="shared" ref="F18" si="8">SUM(F10:F17)</f>
         <v>29114000</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <f t="shared" ref="G18" si="9">SUM(G10:G17)</f>
         <v>29114000</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <f t="shared" ref="H18" si="10">SUM(H10:H17)</f>
         <v>29114000</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="15" t="s">
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="14" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1116,27 +1199,27 @@
         <v>10</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <f>$C$32/$B$20</f>
         <v>3000000</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <f>$C$32/$B$20</f>
         <v>3000000</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <f>$C$32/$B$20</f>
         <v>3000000</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <f>$C$32/$B$20</f>
         <v>3000000</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <f>$C$32/$B$20</f>
         <v>3000000</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="12">
         <f>SUM(D20:H20)</f>
         <v>15000000</v>
       </c>
@@ -1149,21 +1232,21 @@
         <v>0.1</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
         <f>$E$33*$B$21</f>
         <v>3000000</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <f>$E$33*$B$21</f>
         <v>3000000</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <f>$E$33*$B$21</f>
         <v>3000000</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="12">
         <f t="shared" ref="I21:I24" si="11">SUM(D21:H21)</f>
         <v>9000000</v>
       </c>
@@ -1172,31 +1255,31 @@
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>5</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3">
         <f>$C$34/$B$22</f>
         <v>10000000</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <f>$C$34/$B$22</f>
         <v>10000000</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <f>$C$34/$B$22</f>
         <v>10000000</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <f>$C$34/$B$22</f>
         <v>10000000</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="3">
         <f>$C$34/$B$22</f>
         <v>10000000</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="12">
         <f t="shared" si="11"/>
         <v>50000000</v>
       </c>
@@ -1205,56 +1288,56 @@
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>0.2</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="12">
+      <c r="E23" s="3"/>
+      <c r="F23" s="11">
         <f>$E$35*$B$23</f>
         <v>10000000</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="11">
         <f>$E$35*$B$23</f>
         <v>10000000</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="11">
         <f>$E$35*$B$23</f>
         <v>10000000</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="12">
         <f t="shared" si="11"/>
         <v>30000000</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="9">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="8">
         <f>SUM(D20:D23)</f>
         <v>13000000</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <f t="shared" ref="E24:H24" si="12">SUM(E20:E23)</f>
         <v>13000000</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="8">
         <f t="shared" si="12"/>
         <v>26000000</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="8">
         <f t="shared" si="12"/>
         <v>26000000</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="8">
         <f t="shared" si="12"/>
         <v>26000000</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="13">
         <f t="shared" si="11"/>
         <v>104000000</v>
       </c>
@@ -1269,7 +1352,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="17">
+      <c r="H25" s="16">
         <f>I37</f>
         <v>76000000</v>
       </c>
@@ -1280,23 +1363,23 @@
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="12">
+      <c r="D26" s="11">
         <f>D8-D18-D24-D25</f>
         <v>15870000</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="11">
         <f t="shared" ref="E26:H26" si="13">E8-E18-E24-E25</f>
         <v>21690000</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="11">
         <f t="shared" si="13"/>
         <v>24686000</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="11">
         <f t="shared" si="13"/>
         <v>24686000</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="11">
         <f t="shared" si="13"/>
         <v>76686000</v>
       </c>
@@ -1309,50 +1392,50 @@
         <v>0.33</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="12">
+      <c r="D27" s="11">
         <f>D26*$B$27</f>
         <v>5237100</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="11">
         <f t="shared" ref="E27:H27" si="14">E26*$B$27</f>
         <v>7157700</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="11">
         <f t="shared" si="14"/>
         <v>8146380</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="11">
         <f t="shared" si="14"/>
         <v>8146380</v>
       </c>
-      <c r="H27" s="12">
+      <c r="H27" s="11">
         <f t="shared" si="14"/>
         <v>25306380</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="16">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="15">
         <f>D26-D27</f>
         <v>10632900</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="15">
         <f t="shared" ref="E28:H28" si="15">E26-E27</f>
         <v>14532300</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="15">
         <f t="shared" si="15"/>
         <v>16539620</v>
       </c>
-      <c r="G28" s="16">
+      <c r="G28" s="15">
         <f t="shared" si="15"/>
         <v>16539620</v>
       </c>
-      <c r="H28" s="16">
+      <c r="H28" s="15">
         <f t="shared" si="15"/>
         <v>51379620</v>
       </c>
@@ -1367,7 +1450,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="17">
+      <c r="H29" s="16">
         <f>I37</f>
         <v>76000000</v>
       </c>
@@ -1378,39 +1461,39 @@
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="12">
+      <c r="D30" s="11">
         <f>D24</f>
         <v>13000000</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="11">
         <f t="shared" ref="E30:H30" si="16">E24</f>
         <v>13000000</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="11">
         <f t="shared" si="16"/>
         <v>26000000</v>
       </c>
-      <c r="G30" s="12">
+      <c r="G30" s="11">
         <f t="shared" si="16"/>
         <v>26000000</v>
       </c>
-      <c r="H30" s="12">
+      <c r="H30" s="11">
         <f t="shared" si="16"/>
         <v>26000000</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="15" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="14" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1418,10 +1501,10 @@
       <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>30000000</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>30000000</v>
       </c>
       <c r="D32" s="1"/>
@@ -1429,7 +1512,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="13">
+      <c r="I32" s="12">
         <f>C32-I20</f>
         <v>15000000</v>
       </c>
@@ -1438,18 +1521,18 @@
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <v>30000000</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="4">
+      <c r="E33" s="3">
         <v>30000000</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="13">
+      <c r="I33" s="12">
         <f>E33-I21</f>
         <v>21000000</v>
       </c>
@@ -1458,10 +1541,10 @@
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="3">
         <v>50000000</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>50000000</v>
       </c>
       <c r="D34" s="1"/>
@@ -1469,7 +1552,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="13">
+      <c r="I34" s="12">
         <f>C34-I22</f>
         <v>0</v>
       </c>
@@ -1478,18 +1561,18 @@
       <c r="A35" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="3">
         <v>50000000</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="4">
+      <c r="E35" s="3">
         <v>50000000</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="13">
+      <c r="I35" s="12">
         <f>E35-I23</f>
         <v>20000000</v>
       </c>
@@ -1498,10 +1581,10 @@
       <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="3">
         <v>20000000</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="3">
         <v>20000000</v>
       </c>
       <c r="D36" s="1"/>
@@ -1509,71 +1592,71 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="13">
+      <c r="I36" s="12">
         <f>C36</f>
         <v>20000000</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="10">
+      <c r="B37" s="4"/>
+      <c r="C37" s="9">
         <f>SUM(C32:C36)</f>
         <v>100000000</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="9">
         <f t="shared" ref="D37:H37" si="17">SUM(D32:D36)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="9">
         <f t="shared" si="17"/>
         <v>80000000</v>
       </c>
-      <c r="F37" s="10">
+      <c r="F37" s="9">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="G37" s="10">
+      <c r="G37" s="9">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="H37" s="10">
+      <c r="H37" s="9">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="I37" s="18">
+      <c r="I37" s="17">
         <f>SUM(I32:I36)</f>
         <v>76000000</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="20">
+      <c r="B38" s="18"/>
+      <c r="C38" s="19">
         <f>C28+C29+C30-C37</f>
         <v>-100000000</v>
       </c>
-      <c r="D38" s="20">
+      <c r="D38" s="19">
         <f>D28+D29+D30-D37</f>
         <v>23632900</v>
       </c>
-      <c r="E38" s="20">
+      <c r="E38" s="19">
         <f t="shared" ref="E38:H38" si="18">E28+E29+E30-E37</f>
         <v>-52467700</v>
       </c>
-      <c r="F38" s="20">
+      <c r="F38" s="19">
         <f t="shared" si="18"/>
         <v>42539620</v>
       </c>
-      <c r="G38" s="20">
+      <c r="G38" s="19">
         <f t="shared" si="18"/>
         <v>42539620</v>
       </c>
-      <c r="H38" s="20">
+      <c r="H38" s="19">
         <f t="shared" si="18"/>
         <v>153379620</v>
       </c>
@@ -1592,4 +1675,946 @@
   </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D251E8-66D5-3D4B-9E50-31963556F2B3}">
+  <dimension ref="A2:I40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1">
+        <v>30000</v>
+      </c>
+      <c r="E3" s="1">
+        <v>30000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>42000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>42000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>200</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
+        <v>1700</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1900</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1900</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1900</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3">
+        <f>D3*D4</f>
+        <v>51000000</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" ref="E6:G6" si="0">E3*E4</f>
+        <v>57000000</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>79800000</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="0"/>
+        <v>79800000</v>
+      </c>
+      <c r="H6" s="3">
+        <f>H3*H4</f>
+        <v>79800000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3">
+        <v>128000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="8">
+        <f t="shared" ref="D8:H8" si="1">SUM(D6:D7)</f>
+        <v>51000000</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="1"/>
+        <v>57000000</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="1"/>
+        <v>79800000</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="1"/>
+        <v>79800000</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="1"/>
+        <v>207800000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1500000</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="F10" s="3">
+        <v>6500000</v>
+      </c>
+      <c r="G10" s="3">
+        <v>6500000</v>
+      </c>
+      <c r="H10" s="3">
+        <v>6500000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5">
+        <v>150</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3">
+        <f>$B$12*D3</f>
+        <v>4500000</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" ref="E12:H12" si="2">$B$12*E3</f>
+        <v>4500000</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="2"/>
+        <v>6300000</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="2"/>
+        <v>6300000</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="2"/>
+        <v>6300000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5">
+        <v>200</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3">
+        <f>D3*$B$13*IF(D3&gt;40000,90%,100%)</f>
+        <v>6000000</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" ref="E13:H13" si="3">E3*$B$13*IF(E3&gt;40000,90%,100%)</f>
+        <v>6000000</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="3"/>
+        <v>7560000</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="3"/>
+        <v>7560000</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" si="3"/>
+        <v>7560000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5">
+        <v>80</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3">
+        <f>$B$14*D3</f>
+        <v>2400000</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" ref="E14:H14" si="4">$B$14*E3</f>
+        <v>2400000</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="4"/>
+        <v>3360000</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="4"/>
+        <v>3360000</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="4"/>
+        <v>3360000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1500000</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3">
+        <v>1500000</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1500000</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1500000</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1500000</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3">
+        <f>$B$16*D6</f>
+        <v>1530000</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" ref="E16:H16" si="5">$B$16*E6</f>
+        <v>1710000</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="5"/>
+        <v>2394000</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="5"/>
+        <v>2394000</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="5"/>
+        <v>2394000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3">
+        <v>1200000</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1200000</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1500000</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1500000</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8">
+        <f t="shared" ref="D18" si="6">SUM(D10:D17)</f>
+        <v>22130000</v>
+      </c>
+      <c r="E18" s="8">
+        <f t="shared" ref="E18:H18" si="7">SUM(E10:E17)</f>
+        <v>22310000</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="7"/>
+        <v>29114000</v>
+      </c>
+      <c r="G18" s="8">
+        <f t="shared" si="7"/>
+        <v>29114000</v>
+      </c>
+      <c r="H18" s="8">
+        <f t="shared" si="7"/>
+        <v>29114000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="3">
+        <f>$C$34/$B$20</f>
+        <v>3000000</v>
+      </c>
+      <c r="E20" s="3">
+        <f>$C$34/$B$20</f>
+        <v>3000000</v>
+      </c>
+      <c r="F20" s="3">
+        <f>$C$34/$B$20</f>
+        <v>3000000</v>
+      </c>
+      <c r="G20" s="3">
+        <f>$C$34/$B$20</f>
+        <v>3000000</v>
+      </c>
+      <c r="H20" s="3">
+        <f>$C$34/$B$20</f>
+        <v>3000000</v>
+      </c>
+      <c r="I20" s="12">
+        <f>SUM(D20:H20)</f>
+        <v>15000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
+        <f>$E$35*$B$21</f>
+        <v>3000000</v>
+      </c>
+      <c r="G21" s="3">
+        <f>$E$35*$B$21</f>
+        <v>3000000</v>
+      </c>
+      <c r="H21" s="3">
+        <f>$E$35*$B$21</f>
+        <v>3000000</v>
+      </c>
+      <c r="I21" s="12">
+        <f t="shared" ref="I21:I24" si="8">SUM(D21:H21)</f>
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5">
+        <v>5</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3">
+        <f>$C$36/$B$22</f>
+        <v>10000000</v>
+      </c>
+      <c r="E22" s="3">
+        <f>$C$36/$B$22</f>
+        <v>10000000</v>
+      </c>
+      <c r="F22" s="3">
+        <f>$C$36/$B$22</f>
+        <v>10000000</v>
+      </c>
+      <c r="G22" s="3">
+        <f>$C$36/$B$22</f>
+        <v>10000000</v>
+      </c>
+      <c r="H22" s="3">
+        <f>$C$36/$B$22</f>
+        <v>10000000</v>
+      </c>
+      <c r="I22" s="12">
+        <f t="shared" si="8"/>
+        <v>50000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="11">
+        <f>$E$37*$B$23</f>
+        <v>10000000</v>
+      </c>
+      <c r="G23" s="11">
+        <f>$E$37*$B$23</f>
+        <v>10000000</v>
+      </c>
+      <c r="H23" s="11">
+        <f>$E$37*$B$23</f>
+        <v>10000000</v>
+      </c>
+      <c r="I23" s="12">
+        <f t="shared" si="8"/>
+        <v>30000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="8">
+        <f>SUM(D20:D23)</f>
+        <v>13000000</v>
+      </c>
+      <c r="E24" s="8">
+        <f t="shared" ref="E24:H24" si="9">SUM(E20:E23)</f>
+        <v>13000000</v>
+      </c>
+      <c r="F24" s="8">
+        <f t="shared" si="9"/>
+        <v>26000000</v>
+      </c>
+      <c r="G24" s="8">
+        <f t="shared" si="9"/>
+        <v>26000000</v>
+      </c>
+      <c r="H24" s="8">
+        <f t="shared" si="9"/>
+        <v>26000000</v>
+      </c>
+      <c r="I24" s="13">
+        <f t="shared" si="8"/>
+        <v>104000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="16">
+        <f>I39</f>
+        <v>76000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="11">
+        <f>D8-D18-D24-D25</f>
+        <v>15870000</v>
+      </c>
+      <c r="E26" s="11">
+        <f>E8-E18-E24-E25</f>
+        <v>21690000</v>
+      </c>
+      <c r="F26" s="11">
+        <f>F8-F18-F24-F25</f>
+        <v>24686000</v>
+      </c>
+      <c r="G26" s="11">
+        <f>G8-G18-G24-G25</f>
+        <v>24686000</v>
+      </c>
+      <c r="H26" s="11">
+        <f>H8-H18-H24-H25</f>
+        <v>76686000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="11">
+        <f>D8-D18-D24-D25</f>
+        <v>15870000</v>
+      </c>
+      <c r="E28" s="11">
+        <f t="shared" ref="E28:G28" si="10">E8-E18-E24-E25</f>
+        <v>21690000</v>
+      </c>
+      <c r="F28" s="11">
+        <f t="shared" si="10"/>
+        <v>24686000</v>
+      </c>
+      <c r="G28" s="11">
+        <f t="shared" si="10"/>
+        <v>24686000</v>
+      </c>
+      <c r="H28" s="11">
+        <f>H8-H18-H24-H25</f>
+        <v>76686000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="11">
+        <f>D28*$B$29</f>
+        <v>5237100</v>
+      </c>
+      <c r="E29" s="11">
+        <f>E28*$B$29</f>
+        <v>7157700</v>
+      </c>
+      <c r="F29" s="11">
+        <f t="shared" ref="F29:H29" si="11">F28*$B$29</f>
+        <v>8146380</v>
+      </c>
+      <c r="G29" s="11">
+        <f t="shared" si="11"/>
+        <v>8146380</v>
+      </c>
+      <c r="H29" s="11">
+        <f t="shared" si="11"/>
+        <v>25306380</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="15">
+        <f>D26-D29</f>
+        <v>10632900</v>
+      </c>
+      <c r="E30" s="15">
+        <f t="shared" ref="E30:H30" si="12">E26-E29</f>
+        <v>14532300</v>
+      </c>
+      <c r="F30" s="15">
+        <f t="shared" si="12"/>
+        <v>16539620</v>
+      </c>
+      <c r="G30" s="15">
+        <f t="shared" si="12"/>
+        <v>16539620</v>
+      </c>
+      <c r="H30" s="15">
+        <f t="shared" si="12"/>
+        <v>51379620</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="16">
+        <f>I39</f>
+        <v>76000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="11">
+        <f>D24</f>
+        <v>13000000</v>
+      </c>
+      <c r="E32" s="11">
+        <f>E24</f>
+        <v>13000000</v>
+      </c>
+      <c r="F32" s="11">
+        <f>F24</f>
+        <v>26000000</v>
+      </c>
+      <c r="G32" s="11">
+        <f>G24</f>
+        <v>26000000</v>
+      </c>
+      <c r="H32" s="11">
+        <f>H24</f>
+        <v>26000000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="C34" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="12">
+        <f>C34-I20</f>
+        <v>15000000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="12">
+        <f>E35-I21</f>
+        <v>21000000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="3">
+        <v>50000000</v>
+      </c>
+      <c r="C36" s="3">
+        <v>50000000</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="12">
+        <f>C36-I22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="3">
+        <v>50000000</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="3">
+        <v>50000000</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="12">
+        <f>E37-I23</f>
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="3">
+        <v>20000000</v>
+      </c>
+      <c r="C38" s="3">
+        <v>20000000</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="12">
+        <f>C38</f>
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="9">
+        <f>SUM(C34:C38)</f>
+        <v>100000000</v>
+      </c>
+      <c r="D39" s="9">
+        <f t="shared" ref="D39:H39" si="13">SUM(D34:D38)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="9">
+        <f t="shared" si="13"/>
+        <v>80000000</v>
+      </c>
+      <c r="F39" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G39" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="17">
+        <f>SUM(I34:I38)</f>
+        <v>76000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="18"/>
+      <c r="C40" s="19">
+        <f>C30+C31+C32-C39</f>
+        <v>-100000000</v>
+      </c>
+      <c r="D40" s="19">
+        <f>D30+D31+D32-D39</f>
+        <v>23632900</v>
+      </c>
+      <c r="E40" s="19">
+        <f t="shared" ref="E40:H40" si="14">E30+E31+E32-E39</f>
+        <v>-52467700</v>
+      </c>
+      <c r="F40" s="19">
+        <f t="shared" si="14"/>
+        <v>42539620</v>
+      </c>
+      <c r="G40" s="19">
+        <f t="shared" si="14"/>
+        <v>42539620</v>
+      </c>
+      <c r="H40" s="19">
+        <f t="shared" si="14"/>
+        <v>153379620</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A33:H33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>